<commit_message>
fully written draft of the proposal, with a gantt chart of the estimated project timeline
</commit_message>
<xml_diff>
--- a/Writeups/gantt_chart.xlsx
+++ b/Writeups/gantt_chart.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Masters Dissertation Timeline</t>
   </si>
@@ -86,12 +86,6 @@
     <t>Review of methods for verifying user-created rules</t>
   </si>
   <si>
-    <t>Creation of rules</t>
-  </si>
-  <si>
-    <t>Verification</t>
-  </si>
-  <si>
     <t>Benchmarking</t>
   </si>
   <si>
@@ -105,6 +99,18 @@
   </si>
   <si>
     <t>Literature Review</t>
+  </si>
+  <si>
+    <t>Exploring new tactics</t>
+  </si>
+  <si>
+    <t>Close inspection of the behaviour of the prover</t>
+  </si>
+  <si>
+    <t>Comaprison to BEval and other software</t>
+  </si>
+  <si>
+    <t>Response to above/to other things that came up</t>
   </si>
 </sst>
 </file>
@@ -758,11 +764,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AP101"/>
+  <dimension ref="B1:AP103"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +817,7 @@
     <col min="43" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:42" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:42" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="34" t="s">
         <v>0</v>
       </c>
@@ -855,7 +861,7 @@
       <c r="AO1" s="3"/>
       <c r="AP1" s="3"/>
     </row>
-    <row r="2" spans="2:42" s="30" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:42" s="30" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="31" t="s">
         <v>15</v>
       </c>
@@ -900,7 +906,7 @@
       <c r="AO2" s="16"/>
       <c r="AP2" s="16"/>
     </row>
-    <row r="3" spans="2:42" s="30" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:42" s="30" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="29" t="s">
         <v>14</v>
       </c>
@@ -1295,7 +1301,7 @@
     </row>
     <row r="9" spans="2:42" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" s="21">
         <v>15</v>
@@ -1465,7 +1471,7 @@
     </row>
     <row r="15" spans="2:42" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C15" s="21">
         <v>30</v>
@@ -1492,14 +1498,14 @@
       <c r="Y15" s="15"/>
     </row>
     <row r="16" spans="2:42" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
-        <v>20</v>
+      <c r="B16" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="C16" s="21">
         <v>36</v>
       </c>
       <c r="D16" s="21">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E16" s="17"/>
       <c r="F16" s="23"/>
@@ -1521,22 +1527,19 @@
       <c r="AA16" s="18"/>
       <c r="AB16" s="18"/>
       <c r="AC16" s="18"/>
-      <c r="AD16" s="18"/>
-      <c r="AE16" s="18"/>
-      <c r="AF16" s="18"/>
-      <c r="AG16" s="18"/>
-      <c r="AH16" s="18"/>
-      <c r="AI16" s="18"/>
+      <c r="AE16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AI16" s="3"/>
     </row>
     <row r="17" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C17" s="21">
         <v>38</v>
       </c>
       <c r="D17" s="21">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E17" s="17"/>
       <c r="F17" s="23"/>
@@ -1560,14 +1563,12 @@
       <c r="AD17" s="18"/>
       <c r="AE17" s="18"/>
       <c r="AF17" s="18"/>
-      <c r="AG17" s="18"/>
-      <c r="AH17" s="18"/>
-      <c r="AI17" s="18"/>
-      <c r="AJ17" s="18"/>
+      <c r="AG17" s="3"/>
+      <c r="AI17" s="3"/>
     </row>
     <row r="18" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" s="21">
         <v>39</v>
@@ -1599,14 +1600,14 @@
       <c r="AI18" s="3"/>
     </row>
     <row r="19" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
-        <v>22</v>
+      <c r="B19" s="32" t="s">
+        <v>27</v>
       </c>
       <c r="C19" s="21">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D19" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="23"/>
@@ -1624,15 +1625,20 @@
       <c r="W19" s="15"/>
       <c r="X19" s="15"/>
       <c r="Y19" s="15"/>
-      <c r="AK19" s="18"/>
-      <c r="AL19" s="18"/>
+      <c r="AA19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="18"/>
+      <c r="AG19" s="18"/>
+      <c r="AH19" s="18"/>
+      <c r="AI19" s="3"/>
     </row>
     <row r="20" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
-        <v>23</v>
+      <c r="B20" s="32" t="s">
+        <v>28</v>
       </c>
       <c r="C20" s="21">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="D20" s="21">
         <v>3</v>
@@ -1653,19 +1659,23 @@
       <c r="W20" s="15"/>
       <c r="X20" s="15"/>
       <c r="Y20" s="15"/>
-      <c r="AL20" s="18"/>
-      <c r="AM20" s="18"/>
-      <c r="AN20" s="18"/>
+      <c r="AA20" s="3"/>
+      <c r="AC20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="18"/>
+      <c r="AI20" s="18"/>
+      <c r="AJ20" s="18"/>
     </row>
     <row r="21" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="20" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C21" s="21">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D21" s="21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="17"/>
       <c r="F21" s="23"/>
@@ -1683,11 +1693,19 @@
       <c r="W21" s="15"/>
       <c r="X21" s="15"/>
       <c r="Y21" s="15"/>
-      <c r="AO21" s="18"/>
+      <c r="AK21" s="18"/>
+      <c r="AL21" s="18"/>
     </row>
     <row r="22" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
+      <c r="B22" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="21">
+        <v>48</v>
+      </c>
+      <c r="D22" s="21">
+        <v>3</v>
+      </c>
       <c r="E22" s="17"/>
       <c r="F22" s="23"/>
       <c r="G22" s="17"/>
@@ -1704,10 +1722,20 @@
       <c r="W22" s="15"/>
       <c r="X22" s="15"/>
       <c r="Y22" s="15"/>
+      <c r="AL22" s="18"/>
+      <c r="AM22" s="18"/>
+      <c r="AN22" s="18"/>
     </row>
     <row r="23" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="21"/>
-      <c r="D23" s="21"/>
+      <c r="B23" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="21">
+        <v>51</v>
+      </c>
+      <c r="D23" s="21">
+        <v>1</v>
+      </c>
       <c r="E23" s="17"/>
       <c r="F23" s="23"/>
       <c r="G23" s="17"/>
@@ -1724,6 +1752,7 @@
       <c r="W23" s="15"/>
       <c r="X23" s="15"/>
       <c r="Y23" s="15"/>
+      <c r="AO23" s="18"/>
     </row>
     <row r="24" spans="2:41" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="21"/>
@@ -2085,7 +2114,7 @@
       <c r="X41" s="15"/>
       <c r="Y41" s="15"/>
     </row>
-    <row r="42" spans="3:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:25" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
       <c r="E42" s="17"/>
@@ -2101,8 +2130,11 @@
       <c r="T42" s="25"/>
       <c r="U42" s="24"/>
       <c r="V42" s="25"/>
-    </row>
-    <row r="43" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="W42" s="15"/>
+      <c r="X42" s="15"/>
+      <c r="Y42" s="15"/>
+    </row>
+    <row r="43" spans="3:25" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
       <c r="E43" s="17"/>
@@ -2118,6 +2150,9 @@
       <c r="T43" s="25"/>
       <c r="U43" s="24"/>
       <c r="V43" s="25"/>
+      <c r="W43" s="15"/>
+      <c r="X43" s="15"/>
+      <c r="Y43" s="15"/>
     </row>
     <row r="44" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C44" s="21"/>
@@ -2989,10 +3024,36 @@
     <row r="95" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C95" s="21"/>
       <c r="D95" s="21"/>
+      <c r="E95" s="17"/>
+      <c r="F95" s="23"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="23"/>
+      <c r="I95" s="17"/>
+      <c r="J95" s="23"/>
+      <c r="K95" s="17"/>
+      <c r="L95" s="23"/>
+      <c r="M95" s="17"/>
+      <c r="N95" s="28"/>
+      <c r="T95" s="25"/>
+      <c r="U95" s="24"/>
+      <c r="V95" s="25"/>
     </row>
     <row r="96" spans="3:22" x14ac:dyDescent="0.25">
       <c r="C96" s="21"/>
       <c r="D96" s="21"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="23"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="23"/>
+      <c r="I96" s="17"/>
+      <c r="J96" s="23"/>
+      <c r="K96" s="17"/>
+      <c r="L96" s="23"/>
+      <c r="M96" s="17"/>
+      <c r="N96" s="28"/>
+      <c r="T96" s="25"/>
+      <c r="U96" s="24"/>
+      <c r="V96" s="25"/>
     </row>
     <row r="97" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C97" s="21"/>
@@ -3013,6 +3074,14 @@
     <row r="101" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C101" s="21"/>
       <c r="D101" s="21"/>
+    </row>
+    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="21"/>
+      <c r="D102" s="21"/>
+    </row>
+    <row r="103" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="21"/>
+      <c r="D103" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>